<commit_message>
added second data file (STAGE2 coding results)
</commit_message>
<xml_diff>
--- a/data/Data collection for the _orchard plot_ manuscript (Responses)_cleaning2_ML.xlsx
+++ b/data/Data collection for the _orchard plot_ manuscript (Responses)_cleaning2_ML.xlsx
@@ -2175,417 +2175,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="281">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="240">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5204,7 +4794,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A392" sqref="A392:XFD401"/>
+      <selection pane="bottomLeft" activeCell="B402" sqref="B402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -21094,7 +20684,7 @@
         <v>245</v>
       </c>
       <c r="E262" s="3" t="str">
-        <f t="shared" ref="E262:G325" si="575">IF(D262=D263,"same", "diff")</f>
+        <f t="shared" ref="E262:G262" si="575">IF(D262=D263,"same", "diff")</f>
         <v>same</v>
       </c>
       <c r="F262" s="3" t="s">
@@ -29032,7 +28622,7 @@
     </row>
     <row r="399" spans="1:22" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A399" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B399" s="9">
         <v>43781.675978761574</v>
@@ -44673,1202 +44263,1202 @@
     <sortCondition ref="F2:F652"/>
   </sortState>
   <conditionalFormatting sqref="E89:E93 E654:E1048576 E640:E649 E183 E370:E377 E359 E334 E343:E350 E328:E331 E322:E323 E304:E305 E291 E282:E288 E262:E269 E242:E245 E192 E189 E186 E544:E624 E1:E84 E256:E257 G1:G25 J1:J25 M1:M25 P1:P25 S1:S25 V1:V23 E172:E174 E147:E169 E388:E391 E396:E538 G388:G391 J388:J391 M388:M391 P388:P391 S388:S391 V388:V391 E96:E145 G201:G204 E201:E204 J201:J204 M201:M204 P201:P204 S201:S204 V201:V204 J130 G130 M130 P130 S130 V130 E207:E208 E630:E637">
-    <cfRule type="containsText" dxfId="280" priority="281" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="239" priority="281" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J27">
-    <cfRule type="containsText" dxfId="279" priority="267" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="238" priority="267" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89:G93 G654:G1048576 G640:G649 G96:G129 G183 G370:G377 G359 G334 G343:G350 G328:G331 G322:G323 G304:G305 G291 G282:G288 G262:G269 G244 G192 G189 G186 G396:G397 G28:G84 G172:G174 G147:G169 G400:G538 G131:G144 G544:G637">
-    <cfRule type="containsText" dxfId="278" priority="274" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="237" priority="274" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89:J93 J654:J1048576 J640:J649 J96:J129 J183 J370:J377 J359 J334 J343:J350 J328:J331 J322:J323 J304:J305 J291 J282:J288 J262:J269 J244 J192 J189 J186 J544:J625 J396:J397 J28:J84 J172:J174 J147:J169 J400:J538 J131:J144 J630:J637">
-    <cfRule type="containsText" dxfId="40" priority="273" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="236" priority="273" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M89:M93 M654:M1048576 M640:M649 M96:M129 M183 M370:M377 M359 M334 M343:M350 M328:M331 M322:M323 M304:M305 M291 M282:M288 M262:M269 M244 M192 M189 M186 M544:M625 M396:M397 M28:M84 M172:M174 M147:M169 M400:M538 M131:M144 M630:M637">
-    <cfRule type="containsText" dxfId="277" priority="272" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="235" priority="272" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P89:P93 P654:P1048576 P640:P649 P96:P129 P183 P370:P377 P359 P334 P343:P350 P328:P331 P322:P323 P304:P305 P291 P282:P288 P262:P269 P244 P192 P189 P186 P544:P625 P396:P397 P28:P84 P172:P174 P147:P169 P400:P538 P131:P144 P630:P637">
-    <cfRule type="containsText" dxfId="276" priority="271" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="234" priority="271" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S89:S93 S654:S1048576 S640:S649 S96:S129 S183 S370:S377 S359 S334 S343:S350 S328:S331 S322:S323 S304:S305 S291 S282:S288 S262:S269 S244 S192 S189 S186 S544:S625 S396:S397 S28:S84 S172:S174 S147:S169 S400:S538 S131:S144 S630:S637">
-    <cfRule type="containsText" dxfId="275" priority="270" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="233" priority="270" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V24:V25">
-    <cfRule type="containsText" dxfId="274" priority="262" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="232" priority="262" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V89:V93 V654:V1048576 V640:V649 V96:V129 V183 V370:V377 V359 V334 V343:V350 V328:V331 V322:V323 V304:V305 V291 V282:V288 V262:V269 V244 V192 V189 V186 V544:V625 V396:V397 V28:V84 V172:V174 V147:V169 V400:V538 V131:V144 V630:V637">
-    <cfRule type="containsText" dxfId="273" priority="269" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="231" priority="269" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="containsText" dxfId="272" priority="268" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="230" priority="268" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26:M27">
-    <cfRule type="containsText" dxfId="271" priority="266" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="229" priority="266" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26:P27">
-    <cfRule type="containsText" dxfId="270" priority="265" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="228" priority="265" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S26:S27">
-    <cfRule type="containsText" dxfId="269" priority="264" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="227" priority="264" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:V27">
-    <cfRule type="containsText" dxfId="268" priority="263" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="226" priority="263" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V245:V246">
-    <cfRule type="containsText" dxfId="267" priority="207" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="225" priority="207" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S245:S246">
-    <cfRule type="containsText" dxfId="266" priority="208" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="224" priority="208" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G258:G259">
-    <cfRule type="containsText" dxfId="265" priority="260" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="223" priority="260" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G260:G261">
-    <cfRule type="containsText" dxfId="264" priority="259" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="222" priority="259" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G247">
-    <cfRule type="containsText" dxfId="263" priority="258" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="221" priority="258" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G248:G249">
-    <cfRule type="containsText" dxfId="262" priority="257" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="220" priority="257" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G250:G251">
-    <cfRule type="containsText" dxfId="261" priority="256" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="219" priority="256" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G252:G253">
-    <cfRule type="containsText" dxfId="260" priority="255" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="218" priority="255" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G254:G255">
-    <cfRule type="containsText" dxfId="259" priority="254" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="217" priority="254" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G256:G257">
-    <cfRule type="containsText" dxfId="258" priority="253" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="216" priority="253" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J258:J259">
-    <cfRule type="containsText" dxfId="257" priority="252" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="215" priority="252" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J260:J261">
-    <cfRule type="containsText" dxfId="256" priority="251" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="214" priority="251" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J247">
-    <cfRule type="containsText" dxfId="255" priority="250" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="213" priority="250" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J248:J249">
-    <cfRule type="containsText" dxfId="254" priority="249" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="212" priority="249" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J250:J251">
-    <cfRule type="containsText" dxfId="253" priority="248" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="211" priority="248" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J252:J253">
-    <cfRule type="containsText" dxfId="252" priority="247" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="210" priority="247" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J254:J255">
-    <cfRule type="containsText" dxfId="251" priority="246" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="209" priority="246" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J256:J257">
-    <cfRule type="containsText" dxfId="250" priority="245" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="208" priority="245" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M258:M259">
-    <cfRule type="containsText" dxfId="249" priority="244" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="207" priority="244" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M260:M261">
-    <cfRule type="containsText" dxfId="248" priority="243" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="206" priority="243" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M247">
-    <cfRule type="containsText" dxfId="247" priority="242" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="205" priority="242" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M248:M249">
-    <cfRule type="containsText" dxfId="246" priority="241" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="204" priority="241" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M250:M251">
-    <cfRule type="containsText" dxfId="245" priority="240" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="203" priority="240" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M252:M253">
-    <cfRule type="containsText" dxfId="244" priority="239" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="202" priority="239" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M254:M255">
-    <cfRule type="containsText" dxfId="243" priority="238" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="201" priority="238" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M256:M257">
-    <cfRule type="containsText" dxfId="242" priority="237" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="200" priority="237" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P258:P259">
-    <cfRule type="containsText" dxfId="241" priority="236" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="199" priority="236" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P260:P261">
-    <cfRule type="containsText" dxfId="240" priority="235" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="198" priority="235" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P247">
-    <cfRule type="containsText" dxfId="239" priority="234" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="197" priority="234" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P248:P249">
-    <cfRule type="containsText" dxfId="238" priority="233" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="196" priority="233" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P250:P251">
-    <cfRule type="containsText" dxfId="237" priority="232" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="195" priority="232" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P252:P253">
-    <cfRule type="containsText" dxfId="236" priority="231" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="194" priority="231" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P254:P255">
-    <cfRule type="containsText" dxfId="235" priority="230" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="193" priority="230" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P256:P257">
-    <cfRule type="containsText" dxfId="234" priority="229" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="192" priority="229" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S258:S259">
-    <cfRule type="containsText" dxfId="233" priority="228" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="191" priority="228" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S260:S261">
-    <cfRule type="containsText" dxfId="232" priority="227" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="190" priority="227" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S247">
-    <cfRule type="containsText" dxfId="231" priority="226" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="189" priority="226" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S248:S249">
-    <cfRule type="containsText" dxfId="230" priority="225" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="188" priority="225" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S250:S251">
-    <cfRule type="containsText" dxfId="229" priority="224" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="187" priority="224" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S252:S253">
-    <cfRule type="containsText" dxfId="228" priority="223" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="186" priority="223" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S254:S255">
-    <cfRule type="containsText" dxfId="227" priority="222" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="185" priority="222" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S256:S257">
-    <cfRule type="containsText" dxfId="226" priority="221" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="184" priority="221" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V258:V259">
-    <cfRule type="containsText" dxfId="225" priority="220" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="183" priority="220" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V258)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V260:V261">
-    <cfRule type="containsText" dxfId="224" priority="219" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="182" priority="219" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V260)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V247">
-    <cfRule type="containsText" dxfId="223" priority="218" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="181" priority="218" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V248:V249">
-    <cfRule type="containsText" dxfId="222" priority="217" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="180" priority="217" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V250:V251">
-    <cfRule type="containsText" dxfId="221" priority="216" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="179" priority="216" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V252:V253">
-    <cfRule type="containsText" dxfId="220" priority="215" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="178" priority="215" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V254:V255">
-    <cfRule type="containsText" dxfId="219" priority="214" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="177" priority="214" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V254)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V256:V257">
-    <cfRule type="containsText" dxfId="218" priority="213" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="176" priority="213" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V256)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G245:G246">
-    <cfRule type="containsText" dxfId="217" priority="212" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="175" priority="212" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J245:J246">
-    <cfRule type="containsText" dxfId="216" priority="211" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="174" priority="211" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M245:M246">
-    <cfRule type="containsText" dxfId="215" priority="210" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="173" priority="210" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P245:P246">
-    <cfRule type="containsText" dxfId="214" priority="209" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="172" priority="209" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E146">
-    <cfRule type="containsText" dxfId="213" priority="199" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="171" priority="199" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S145:S146">
-    <cfRule type="containsText" dxfId="212" priority="188" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="170" priority="188" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V145:V146">
-    <cfRule type="containsText" dxfId="211" priority="187" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="169" priority="187" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G145:G146">
-    <cfRule type="containsText" dxfId="210" priority="191" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="168" priority="191" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J145:J146">
-    <cfRule type="containsText" dxfId="209" priority="192" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="167" priority="192" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M145:M146">
-    <cfRule type="containsText" dxfId="208" priority="190" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="166" priority="190" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P145:P146">
-    <cfRule type="containsText" dxfId="207" priority="189" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="165" priority="189" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G398:G399">
-    <cfRule type="containsText" dxfId="206" priority="186" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="164" priority="186" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J398:J399">
-    <cfRule type="containsText" dxfId="205" priority="185" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="163" priority="185" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P398:P399">
-    <cfRule type="containsText" dxfId="204" priority="184" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="162" priority="184" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M398:M399">
-    <cfRule type="containsText" dxfId="203" priority="183" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="161" priority="183" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S398:S399">
-    <cfRule type="containsText" dxfId="202" priority="182" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="160" priority="182" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V398:V399">
-    <cfRule type="containsText" dxfId="201" priority="181" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="159" priority="181" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E170:E171">
-    <cfRule type="containsText" dxfId="200" priority="167" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="158" priority="167" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J170:J171">
-    <cfRule type="containsText" dxfId="199" priority="165" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="157" priority="165" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G170:G171">
-    <cfRule type="containsText" dxfId="198" priority="166" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="156" priority="166" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V170:V171">
-    <cfRule type="containsText" dxfId="197" priority="161" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="155" priority="161" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M170:M171">
-    <cfRule type="containsText" dxfId="196" priority="164" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="154" priority="164" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P170:P171">
-    <cfRule type="containsText" dxfId="195" priority="163" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="153" priority="163" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S170:S171">
-    <cfRule type="containsText" dxfId="194" priority="162" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="152" priority="162" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S170)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E205:E206">
-    <cfRule type="containsText" dxfId="191" priority="152" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="151" priority="152" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E209:E210">
-    <cfRule type="containsText" dxfId="190" priority="151" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="150" priority="151" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E211">
-    <cfRule type="containsText" dxfId="189" priority="150" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="149" priority="150" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E212:E213">
-    <cfRule type="containsText" dxfId="188" priority="149" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="148" priority="149" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E214:E215">
-    <cfRule type="containsText" dxfId="187" priority="148" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="147" priority="148" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E216:E217">
-    <cfRule type="containsText" dxfId="186" priority="147" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="146" priority="147" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E218:E219">
-    <cfRule type="containsText" dxfId="185" priority="146" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="145" priority="146" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E220:E221">
-    <cfRule type="containsText" dxfId="184" priority="145" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="144" priority="145" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E222:E223">
-    <cfRule type="containsText" dxfId="183" priority="144" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="143" priority="144" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E224:E225">
-    <cfRule type="containsText" dxfId="182" priority="143" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="142" priority="143" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E226:E227">
-    <cfRule type="containsText" dxfId="181" priority="142" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="141" priority="142" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E228:E229">
-    <cfRule type="containsText" dxfId="180" priority="141" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="140" priority="141" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E230:E231">
-    <cfRule type="containsText" dxfId="179" priority="140" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E232">
-    <cfRule type="containsText" dxfId="178" priority="139" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="138" priority="139" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E235:E236">
-    <cfRule type="containsText" dxfId="177" priority="138" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="137" priority="138" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E233:E234">
-    <cfRule type="containsText" dxfId="176" priority="137" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="136" priority="137" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E237">
-    <cfRule type="containsText" dxfId="175" priority="136" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="135" priority="136" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E238:E239">
-    <cfRule type="containsText" dxfId="174" priority="135" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="134" priority="135" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E240:E241">
-    <cfRule type="containsText" dxfId="173" priority="134" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G242:G243 G207:G208">
-    <cfRule type="containsText" dxfId="172" priority="133" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="132" priority="133" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206">
-    <cfRule type="containsText" dxfId="171" priority="132" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="131" priority="132" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G209:G210">
-    <cfRule type="containsText" dxfId="170" priority="131" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G211">
-    <cfRule type="containsText" dxfId="169" priority="130" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="129" priority="130" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212:G213">
-    <cfRule type="containsText" dxfId="168" priority="129" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="128" priority="129" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G214:G215">
-    <cfRule type="containsText" dxfId="167" priority="128" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G216:G217">
-    <cfRule type="containsText" dxfId="166" priority="127" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="126" priority="127" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G218:G219">
-    <cfRule type="containsText" dxfId="165" priority="126" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="125" priority="126" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G220:G221">
-    <cfRule type="containsText" dxfId="164" priority="125" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G222:G223">
-    <cfRule type="containsText" dxfId="163" priority="124" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="123" priority="124" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G224:G225">
-    <cfRule type="containsText" dxfId="162" priority="123" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="122" priority="123" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G226:G227">
-    <cfRule type="containsText" dxfId="161" priority="122" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G228:G229">
-    <cfRule type="containsText" dxfId="160" priority="121" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="120" priority="121" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G230:G231">
-    <cfRule type="containsText" dxfId="159" priority="120" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="119" priority="120" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G232">
-    <cfRule type="containsText" dxfId="158" priority="119" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G235:G236">
-    <cfRule type="containsText" dxfId="157" priority="118" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="117" priority="118" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G233:G234">
-    <cfRule type="containsText" dxfId="156" priority="117" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="116" priority="117" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G237">
-    <cfRule type="containsText" dxfId="155" priority="116" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G238:G239">
-    <cfRule type="containsText" dxfId="154" priority="115" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="114" priority="115" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G240:G241">
-    <cfRule type="containsText" dxfId="153" priority="114" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="113" priority="114" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",G240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J242:J243 J207:J208">
-    <cfRule type="containsText" dxfId="152" priority="113" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J206">
-    <cfRule type="containsText" dxfId="151" priority="112" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="111" priority="112" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J209:J210">
-    <cfRule type="containsText" dxfId="150" priority="111" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="110" priority="111" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J211">
-    <cfRule type="containsText" dxfId="149" priority="110" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J212:J213">
-    <cfRule type="containsText" dxfId="148" priority="109" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="108" priority="109" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J214:J215">
-    <cfRule type="containsText" dxfId="147" priority="108" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="107" priority="108" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J216:J217">
-    <cfRule type="containsText" dxfId="146" priority="107" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J218:J219">
-    <cfRule type="containsText" dxfId="145" priority="106" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="105" priority="106" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J220:J221">
-    <cfRule type="containsText" dxfId="144" priority="105" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="104" priority="105" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J222:J223">
-    <cfRule type="containsText" dxfId="143" priority="104" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J224:J225">
-    <cfRule type="containsText" dxfId="142" priority="103" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="102" priority="103" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J226:J227">
-    <cfRule type="containsText" dxfId="141" priority="102" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="101" priority="102" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J228:J229">
-    <cfRule type="containsText" dxfId="140" priority="101" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J230:J231">
-    <cfRule type="containsText" dxfId="139" priority="100" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J232">
-    <cfRule type="containsText" dxfId="138" priority="99" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="98" priority="99" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J235:J236">
-    <cfRule type="containsText" dxfId="137" priority="98" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J233:J234">
-    <cfRule type="containsText" dxfId="136" priority="97" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="96" priority="97" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J237">
-    <cfRule type="containsText" dxfId="135" priority="96" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="95" priority="96" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J238:J239">
-    <cfRule type="containsText" dxfId="134" priority="95" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J240:J241">
-    <cfRule type="containsText" dxfId="133" priority="94" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="93" priority="94" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M242:M243 M207:M208">
-    <cfRule type="containsText" dxfId="132" priority="93" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="92" priority="93" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M206">
-    <cfRule type="containsText" dxfId="131" priority="92" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M209:M210">
-    <cfRule type="containsText" dxfId="130" priority="91" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="90" priority="91" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M211">
-    <cfRule type="containsText" dxfId="129" priority="90" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M212:M213">
-    <cfRule type="containsText" dxfId="128" priority="89" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M214:M215">
-    <cfRule type="containsText" dxfId="127" priority="88" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M216:M217">
-    <cfRule type="containsText" dxfId="126" priority="87" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M218:M219">
-    <cfRule type="containsText" dxfId="125" priority="86" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M220:M221">
-    <cfRule type="containsText" dxfId="124" priority="85" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M222:M223">
-    <cfRule type="containsText" dxfId="123" priority="84" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="83" priority="84" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M224:M225">
-    <cfRule type="containsText" dxfId="122" priority="83" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M226:M227">
-    <cfRule type="containsText" dxfId="121" priority="82" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="81" priority="82" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M228:M229">
-    <cfRule type="containsText" dxfId="120" priority="81" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M230:M231">
-    <cfRule type="containsText" dxfId="119" priority="80" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M232">
-    <cfRule type="containsText" dxfId="118" priority="79" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M235:M236">
-    <cfRule type="containsText" dxfId="117" priority="78" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M233:M234">
-    <cfRule type="containsText" dxfId="116" priority="77" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M237">
-    <cfRule type="containsText" dxfId="115" priority="76" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M238:M239">
-    <cfRule type="containsText" dxfId="114" priority="75" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M240:M241">
-    <cfRule type="containsText" dxfId="113" priority="74" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P242:P243 P207:P208">
-    <cfRule type="containsText" dxfId="112" priority="73" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P206">
-    <cfRule type="containsText" dxfId="111" priority="72" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P209:P210">
-    <cfRule type="containsText" dxfId="110" priority="71" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P211">
-    <cfRule type="containsText" dxfId="109" priority="70" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P212:P213">
-    <cfRule type="containsText" dxfId="108" priority="69" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P214:P215">
-    <cfRule type="containsText" dxfId="107" priority="68" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P216:P217">
-    <cfRule type="containsText" dxfId="106" priority="67" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P218:P219">
-    <cfRule type="containsText" dxfId="105" priority="66" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P220:P221">
-    <cfRule type="containsText" dxfId="104" priority="65" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P222:P223">
-    <cfRule type="containsText" dxfId="103" priority="64" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P224:P225">
-    <cfRule type="containsText" dxfId="102" priority="63" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P226:P227">
-    <cfRule type="containsText" dxfId="101" priority="62" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P228:P229">
-    <cfRule type="containsText" dxfId="100" priority="61" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P230:P231">
-    <cfRule type="containsText" dxfId="99" priority="60" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P232">
-    <cfRule type="containsText" dxfId="98" priority="59" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P235:P236">
-    <cfRule type="containsText" dxfId="97" priority="58" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P233:P234">
-    <cfRule type="containsText" dxfId="96" priority="57" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P237">
-    <cfRule type="containsText" dxfId="95" priority="56" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P238:P239">
-    <cfRule type="containsText" dxfId="94" priority="55" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P240:P241">
-    <cfRule type="containsText" dxfId="93" priority="54" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S242:S243 S207:S208">
-    <cfRule type="containsText" dxfId="92" priority="53" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S206">
-    <cfRule type="containsText" dxfId="91" priority="52" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S209:S210">
-    <cfRule type="containsText" dxfId="90" priority="51" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S211">
-    <cfRule type="containsText" dxfId="89" priority="50" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S212:S213">
-    <cfRule type="containsText" dxfId="88" priority="49" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S214:S215">
-    <cfRule type="containsText" dxfId="87" priority="48" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S216:S217">
-    <cfRule type="containsText" dxfId="86" priority="47" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S218:S219">
-    <cfRule type="containsText" dxfId="85" priority="46" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S220:S221">
-    <cfRule type="containsText" dxfId="84" priority="45" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S222:S223">
-    <cfRule type="containsText" dxfId="83" priority="44" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S224:S225">
-    <cfRule type="containsText" dxfId="82" priority="43" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S226:S227">
-    <cfRule type="containsText" dxfId="81" priority="42" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S228:S229">
-    <cfRule type="containsText" dxfId="80" priority="41" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S230:S231">
-    <cfRule type="containsText" dxfId="79" priority="40" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S232">
-    <cfRule type="containsText" dxfId="78" priority="39" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S235:S236">
-    <cfRule type="containsText" dxfId="77" priority="38" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S233:S234">
-    <cfRule type="containsText" dxfId="76" priority="37" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S237">
-    <cfRule type="containsText" dxfId="75" priority="36" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S238:S239">
-    <cfRule type="containsText" dxfId="74" priority="35" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S240:S241">
-    <cfRule type="containsText" dxfId="73" priority="34" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V242:V243 V207:V208">
-    <cfRule type="containsText" dxfId="72" priority="33" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V206">
-    <cfRule type="containsText" dxfId="71" priority="32" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V209:V210">
-    <cfRule type="containsText" dxfId="70" priority="31" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V211">
-    <cfRule type="containsText" dxfId="69" priority="30" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V212:V213">
-    <cfRule type="containsText" dxfId="68" priority="29" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V212)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V214:V215">
-    <cfRule type="containsText" dxfId="67" priority="28" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V216:V217">
-    <cfRule type="containsText" dxfId="66" priority="27" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V218:V219">
-    <cfRule type="containsText" dxfId="65" priority="26" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V220:V221">
-    <cfRule type="containsText" dxfId="64" priority="25" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V222:V223">
-    <cfRule type="containsText" dxfId="63" priority="24" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V224:V225">
-    <cfRule type="containsText" dxfId="62" priority="23" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V224)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V226:V227">
-    <cfRule type="containsText" dxfId="61" priority="22" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V228:V229">
-    <cfRule type="containsText" dxfId="60" priority="21" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V230:V231">
-    <cfRule type="containsText" dxfId="59" priority="20" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V232">
-    <cfRule type="containsText" dxfId="58" priority="19" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V235:V236">
-    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V233:V234">
-    <cfRule type="containsText" dxfId="56" priority="17" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V237">
-    <cfRule type="containsText" dxfId="55" priority="16" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V238:V239">
-    <cfRule type="containsText" dxfId="54" priority="15" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V240:V241">
-    <cfRule type="containsText" dxfId="53" priority="14" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J626">
-    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J627">
-    <cfRule type="containsText" dxfId="51" priority="12" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J627)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J628">
-    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J628)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J629">
-    <cfRule type="containsText" dxfId="49" priority="10" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",J629)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M626:M629">
-    <cfRule type="containsText" dxfId="48" priority="9" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P626:P629">
-    <cfRule type="containsText" dxfId="47" priority="8" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S626:S629">
-    <cfRule type="containsText" dxfId="46" priority="7" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",S626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V626:V629">
-    <cfRule type="containsText" dxfId="45" priority="6" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",V626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E626:E629">
-    <cfRule type="containsText" dxfId="44" priority="5" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E625">
-    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",E625)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P360:P364">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P360)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P365:P369">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",P365)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M368:M369">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="diff">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="diff">
       <formula>NOT(ISERROR(SEARCH("diff",M368)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>